<commit_message>
Output files have changed because of the changes made to the scripts generating them
</commit_message>
<xml_diff>
--- a/data/list_of_studies_by_council.xlsx
+++ b/data/list_of_studies_by_council.xlsx
@@ -19,49 +19,49 @@
     <t>Case Study Id</t>
   </si>
   <si>
-    <t>ahrc</t>
+    <t>funder_ahrc</t>
   </si>
   <si>
-    <t>bbsrc</t>
+    <t>funder_bbsrc</t>
   </si>
   <si>
-    <t>british_academy</t>
+    <t>funder_british_academy</t>
   </si>
   <si>
-    <t>cclrc</t>
+    <t>funder_cclrc</t>
   </si>
   <si>
-    <t>epsrc</t>
+    <t>funder_epsrc</t>
   </si>
   <si>
-    <t>esrc</t>
+    <t>funder_esrc</t>
   </si>
   <si>
-    <t>mrc</t>
+    <t>funder_mrc</t>
   </si>
   <si>
-    <t>nerc</t>
+    <t>funder_nerc</t>
   </si>
   <si>
-    <t>pparc</t>
+    <t>funder_pparc</t>
   </si>
   <si>
-    <t>rcuk</t>
+    <t>funder_rcuk</t>
   </si>
   <si>
-    <t>royal_academy_engineering</t>
+    <t>funder_royal_academy_engineering</t>
   </si>
   <si>
-    <t>royal_society</t>
+    <t>funder_royal_society</t>
   </si>
   <si>
-    <t>stfc</t>
+    <t>funder_stfc</t>
   </si>
   <si>
-    <t>uk_space_agency</t>
+    <t>funder_uk_space_agency</t>
   </si>
   <si>
-    <t>wellcome</t>
+    <t>funder_wellcome</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3563"/>
+  <dimension ref="A1:P3562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -81908,24 +81908,6 @@
       <c r="O3562" t="s"/>
       <c r="P3562" t="s"/>
     </row>
-    <row r="3563" spans="1:16">
-      <c r="A3563" s="1" t="s"/>
-      <c r="B3563" t="s"/>
-      <c r="C3563" t="s"/>
-      <c r="D3563" t="s"/>
-      <c r="E3563" t="s"/>
-      <c r="F3563" t="s"/>
-      <c r="G3563" t="s"/>
-      <c r="H3563" t="s"/>
-      <c r="I3563" t="s"/>
-      <c r="J3563" t="s"/>
-      <c r="K3563" t="s"/>
-      <c r="L3563" t="s"/>
-      <c r="M3563" t="s"/>
-      <c r="N3563" t="s"/>
-      <c r="O3563" t="s"/>
-      <c r="P3563" t="s"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>